<commit_message>
Xong gui mail diem + SK
</commit_message>
<xml_diff>
--- a/src/upload/Mau_Nhap_Diem_Lop_1.xlsx
+++ b/src/upload/Mau_Nhap_Diem_Lop_1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huynh\Desktop\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyPC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="20">
   <si>
     <t>STT</t>
   </si>
@@ -67,6 +67,9 @@
   </si>
   <si>
     <t>Tran Minh Loc edited</t>
+  </si>
+  <si>
+    <t>D</t>
   </si>
   <si>
     <t>T</t>
@@ -81,12 +84,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -455,27 +458,26 @@
   <dimension ref="A1:M4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="J6" sqref="J6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="4.88671875" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="8.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="14.33203125" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="7.44140625" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="9.109375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -516,7 +518,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A2">
         <v>1</v>
       </c>
@@ -527,7 +529,7 @@
         <v>13</v>
       </c>
       <c r="D2">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="E2">
         <v>8</v>
@@ -536,28 +538,28 @@
         <v>9</v>
       </c>
       <c r="G2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="H2">
         <v>9</v>
       </c>
       <c r="I2">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="J2" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="K2" t="s">
         <v>16</v>
       </c>
       <c r="L2" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M2" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>2</v>
       </c>
@@ -568,37 +570,37 @@
         <v>14</v>
       </c>
       <c r="D3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="E3">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="F3">
         <v>8</v>
       </c>
       <c r="G3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="H3">
         <v>8</v>
       </c>
       <c r="I3">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="J3" t="s">
         <v>16</v>
       </c>
       <c r="K3" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="L3" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" ht="15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>3</v>
       </c>
@@ -609,34 +611,34 @@
         <v>15</v>
       </c>
       <c r="D4">
-        <v>9</v>
+        <v>8</v>
       </c>
       <c r="E4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="F4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="G4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="H4">
-        <v>7</v>
+        <v>9</v>
       </c>
       <c r="I4">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="J4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="K4" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="L4" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="M4" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
xong 1 phan nhap diem
</commit_message>
<xml_diff>
--- a/src/upload/Mau_Nhap_Diem_Lop_1.xlsx
+++ b/src/upload/Mau_Nhap_Diem_Lop_1.xlsx
@@ -5,11 +5,11 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\huynh\Desktop\Excel\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyPC\Desktop\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7755"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="20490" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="sheet1" sheetId="1" r:id="rId1"/>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="19">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="21">
   <si>
     <t>STT</t>
   </si>
@@ -60,6 +60,12 @@
     <t>Nhận Xét Của Giáo Viên</t>
   </si>
   <si>
+    <t>Điểm</t>
+  </si>
+  <si>
+    <t>Nhận Xét</t>
+  </si>
+  <si>
     <t>Nguyen Huynh Duc</t>
   </si>
   <si>
@@ -72,7 +78,7 @@
     <t>T</t>
   </si>
   <si>
-    <t>K</t>
+    <t>Tốt</t>
   </si>
   <si>
     <t>Chăm ngoan học giỏi</t>
@@ -81,12 +87,12 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
+      <name val="Arial"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
@@ -111,7 +117,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="3">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
@@ -452,30 +460,39 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:M4"/>
+  <dimension ref="A1:V6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
+      <selection activeCell="V9" sqref="V9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="3.75" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="18.25" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="4.875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="9.125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="8" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="16.125" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.25" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="7.5" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="8.125" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="9.25" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="20.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="17.44140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="5.21875" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="8.109375" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -485,164 +502,324 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="2"/>
+      <c r="F1" s="2" t="s">
         <v>4</v>
       </c>
-      <c r="F1" t="s">
+      <c r="G1" s="2"/>
+      <c r="H1" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="G1" t="s">
+      <c r="I1" s="2"/>
+      <c r="J1" s="2" t="s">
         <v>6</v>
       </c>
-      <c r="H1" t="s">
+      <c r="K1" s="2"/>
+      <c r="L1" s="2" t="s">
         <v>7</v>
       </c>
-      <c r="I1" t="s">
+      <c r="M1" s="2"/>
+      <c r="N1" s="2" t="s">
         <v>8</v>
       </c>
-      <c r="J1" t="s">
+      <c r="O1" s="2"/>
+      <c r="P1" s="2" t="s">
         <v>9</v>
       </c>
-      <c r="K1" t="s">
+      <c r="Q1" s="2"/>
+      <c r="R1" s="2" t="s">
         <v>10</v>
       </c>
-      <c r="L1" t="s">
+      <c r="S1" s="2"/>
+      <c r="T1" s="2" t="s">
         <v>11</v>
       </c>
-      <c r="M1" t="s">
+      <c r="U1" s="2"/>
+      <c r="V1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A2">
+    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="D2" t="s">
+        <v>13</v>
+      </c>
+      <c r="E2" t="s">
+        <v>14</v>
+      </c>
+      <c r="F2" t="s">
+        <v>13</v>
+      </c>
+      <c r="G2" t="s">
+        <v>14</v>
+      </c>
+      <c r="H2" t="s">
+        <v>13</v>
+      </c>
+      <c r="I2" t="s">
+        <v>14</v>
+      </c>
+      <c r="J2" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" t="s">
+        <v>14</v>
+      </c>
+      <c r="L2" t="s">
+        <v>13</v>
+      </c>
+      <c r="M2" t="s">
+        <v>14</v>
+      </c>
+      <c r="N2" t="s">
+        <v>13</v>
+      </c>
+      <c r="O2" t="s">
+        <v>14</v>
+      </c>
+      <c r="P2" t="s">
+        <v>13</v>
+      </c>
+      <c r="Q2" t="s">
+        <v>14</v>
+      </c>
+      <c r="R2" t="s">
+        <v>13</v>
+      </c>
+      <c r="S2" t="s">
+        <v>14</v>
+      </c>
+      <c r="T2" t="s">
+        <v>13</v>
+      </c>
+      <c r="U2" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A3">
         <v>1</v>
       </c>
-      <c r="B2">
+      <c r="B3">
         <v>16</v>
       </c>
-      <c r="C2" t="s">
-        <v>13</v>
-      </c>
-      <c r="D2">
-        <v>7</v>
-      </c>
-      <c r="E2">
-        <v>8</v>
-      </c>
-      <c r="F2">
+      <c r="C3" t="s">
+        <v>15</v>
+      </c>
+      <c r="D3">
         <v>9</v>
       </c>
-      <c r="G2">
-        <v>9</v>
-      </c>
-      <c r="H2">
-        <v>9</v>
-      </c>
-      <c r="I2">
-        <v>9</v>
-      </c>
-      <c r="J2" t="s">
-        <v>16</v>
-      </c>
-      <c r="K2" t="s">
-        <v>16</v>
-      </c>
-      <c r="L2" t="s">
-        <v>16</v>
-      </c>
-      <c r="M2" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="3" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A3">
-        <v>2</v>
-      </c>
-      <c r="B3">
-        <v>23</v>
-      </c>
-      <c r="C3" t="s">
-        <v>14</v>
-      </c>
-      <c r="D3">
-        <v>8</v>
-      </c>
-      <c r="E3">
-        <v>9</v>
+      <c r="E3" t="s">
+        <v>19</v>
       </c>
       <c r="F3">
         <v>8</v>
       </c>
-      <c r="G3">
+      <c r="G3" t="s">
+        <v>19</v>
+      </c>
+      <c r="H3" t="s">
+        <v>18</v>
+      </c>
+      <c r="I3" t="s">
+        <v>19</v>
+      </c>
+      <c r="J3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K3" t="s">
+        <v>19</v>
+      </c>
+      <c r="L3" t="s">
+        <v>18</v>
+      </c>
+      <c r="M3" t="s">
+        <v>19</v>
+      </c>
+      <c r="N3" t="s">
+        <v>18</v>
+      </c>
+      <c r="O3" t="s">
+        <v>19</v>
+      </c>
+      <c r="P3" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q3" t="s">
+        <v>19</v>
+      </c>
+      <c r="R3" t="s">
+        <v>18</v>
+      </c>
+      <c r="S3" t="s">
+        <v>19</v>
+      </c>
+      <c r="T3" t="s">
+        <v>18</v>
+      </c>
+      <c r="U3" t="s">
+        <v>19</v>
+      </c>
+      <c r="V3" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A4">
+        <v>2</v>
+      </c>
+      <c r="B4">
+        <v>23</v>
+      </c>
+      <c r="C4" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4">
         <v>8</v>
       </c>
-      <c r="H3">
+      <c r="E4" t="s">
+        <v>19</v>
+      </c>
+      <c r="F4">
+        <v>9</v>
+      </c>
+      <c r="G4" t="s">
+        <v>19</v>
+      </c>
+      <c r="H4" t="s">
+        <v>18</v>
+      </c>
+      <c r="I4" t="s">
+        <v>19</v>
+      </c>
+      <c r="J4" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="s">
+        <v>19</v>
+      </c>
+      <c r="L4" t="s">
+        <v>18</v>
+      </c>
+      <c r="M4" t="s">
+        <v>19</v>
+      </c>
+      <c r="N4" t="s">
+        <v>18</v>
+      </c>
+      <c r="O4" t="s">
+        <v>19</v>
+      </c>
+      <c r="P4" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q4" t="s">
+        <v>19</v>
+      </c>
+      <c r="R4" t="s">
+        <v>18</v>
+      </c>
+      <c r="S4" t="s">
+        <v>19</v>
+      </c>
+      <c r="T4" t="s">
+        <v>18</v>
+      </c>
+      <c r="U4" t="s">
+        <v>19</v>
+      </c>
+      <c r="V4" s="1" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="A5">
+        <v>3</v>
+      </c>
+      <c r="B5">
+        <v>25</v>
+      </c>
+      <c r="C5" t="s">
+        <v>17</v>
+      </c>
+      <c r="D5">
+        <v>9</v>
+      </c>
+      <c r="E5" t="s">
+        <v>19</v>
+      </c>
+      <c r="F5">
         <v>8</v>
       </c>
-      <c r="I3">
-        <v>8</v>
-      </c>
-      <c r="J3" t="s">
-        <v>16</v>
-      </c>
-      <c r="K3" t="s">
-        <v>16</v>
-      </c>
-      <c r="L3" t="s">
-        <v>17</v>
-      </c>
-      <c r="M3" t="s">
-        <v>18</v>
+      <c r="G5" t="s">
+        <v>19</v>
+      </c>
+      <c r="H5" t="s">
+        <v>18</v>
+      </c>
+      <c r="I5" t="s">
+        <v>19</v>
+      </c>
+      <c r="J5" t="s">
+        <v>18</v>
+      </c>
+      <c r="K5" t="s">
+        <v>19</v>
+      </c>
+      <c r="L5" t="s">
+        <v>18</v>
+      </c>
+      <c r="M5" t="s">
+        <v>19</v>
+      </c>
+      <c r="N5" t="s">
+        <v>18</v>
+      </c>
+      <c r="O5" t="s">
+        <v>19</v>
+      </c>
+      <c r="P5" t="s">
+        <v>18</v>
+      </c>
+      <c r="Q5" t="s">
+        <v>19</v>
+      </c>
+      <c r="R5" t="s">
+        <v>18</v>
+      </c>
+      <c r="S5" t="s">
+        <v>19</v>
+      </c>
+      <c r="T5" t="s">
+        <v>18</v>
+      </c>
+      <c r="U5" t="s">
+        <v>19</v>
+      </c>
+      <c r="V5" s="1" t="s">
+        <v>20</v>
       </c>
     </row>
-    <row r="4" spans="1:13" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A4">
-        <v>3</v>
-      </c>
-      <c r="B4">
-        <v>25</v>
-      </c>
-      <c r="C4" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4">
-        <v>9</v>
-      </c>
-      <c r="E4">
-        <v>7</v>
-      </c>
-      <c r="F4">
-        <v>7</v>
-      </c>
-      <c r="G4">
-        <v>7</v>
-      </c>
-      <c r="H4">
-        <v>7</v>
-      </c>
-      <c r="I4">
-        <v>7</v>
-      </c>
-      <c r="J4" t="s">
-        <v>16</v>
-      </c>
-      <c r="K4" t="s">
-        <v>16</v>
-      </c>
-      <c r="L4" t="s">
-        <v>16</v>
-      </c>
-      <c r="M4" t="s">
-        <v>18</v>
-      </c>
+    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
+      <c r="V6" s="1"/>
     </row>
   </sheetData>
+  <mergeCells count="9">
+    <mergeCell ref="N1:O1"/>
+    <mergeCell ref="P1:Q1"/>
+    <mergeCell ref="R1:S1"/>
+    <mergeCell ref="T1:U1"/>
+    <mergeCell ref="D1:E1"/>
+    <mergeCell ref="F1:G1"/>
+    <mergeCell ref="H1:I1"/>
+    <mergeCell ref="J1:K1"/>
+    <mergeCell ref="L1:M1"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <ignoredErrors>
-    <ignoredError sqref="A1:M1 A4:C4 A2:C2 A3:C3" numberStoredAsText="1"/>
+    <ignoredError sqref="A1:V2 A5:C5 A3:C3 A4:C4" numberStoredAsText="1"/>
   </ignoredErrors>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
ban cuoi truoc khi nop LV
</commit_message>
<xml_diff>
--- a/src/upload/Mau_Nhap_Diem_Lop_1.xlsx
+++ b/src/upload/Mau_Nhap_Diem_Lop_1.xlsx
@@ -5,7 +5,7 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyPC\Desktop\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\MyPC\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="85" uniqueCount="35">
   <si>
     <t>STT</t>
   </si>
@@ -78,10 +78,52 @@
     <t>T</t>
   </si>
   <si>
-    <t>Tốt</t>
-  </si>
-  <si>
-    <t>Chăm ngoan học giỏi</t>
+    <t>Cháu học nhanh hiểu</t>
+  </si>
+  <si>
+    <t>Cháu còn chậm hiểu</t>
+  </si>
+  <si>
+    <t>Cháo hoàn thành tốt môn học</t>
+  </si>
+  <si>
+    <t>Cháu đọc bài to, rõ</t>
+  </si>
+  <si>
+    <t>Cháo đọc chữ chưa chạy</t>
+  </si>
+  <si>
+    <t>Cháo đọc bài còn kém</t>
+  </si>
+  <si>
+    <t>Cháu hoàn thành tốt</t>
+  </si>
+  <si>
+    <t>Cháu ham học hỏi</t>
+  </si>
+  <si>
+    <t>Cháu còn nhút nhát</t>
+  </si>
+  <si>
+    <t>Cháu năng động trong lớp</t>
+  </si>
+  <si>
+    <t>Cháo nhanh tiếp thu</t>
+  </si>
+  <si>
+    <t>Cháu nhanh nhớ bài</t>
+  </si>
+  <si>
+    <t>Cháu chưa thuộc bài nhiều</t>
+  </si>
+  <si>
+    <t>Cháu hát to, tự tin</t>
+  </si>
+  <si>
+    <t>Cháu hát tốt</t>
+  </si>
+  <si>
+    <t>Chăn ngoan học giỏi</t>
   </si>
 </sst>
 </file>
@@ -117,8 +159,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
@@ -460,13 +501,13 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:V6"/>
+  <dimension ref="A1:V5"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="D1" workbookViewId="0">
-      <selection activeCell="V9" sqref="V9"/>
+    <sheetView tabSelected="1" topLeftCell="C1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <selection activeCell="Q11" sqref="Q11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="14.25" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="4.21875" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.6640625" bestFit="1" customWidth="1"/>
@@ -492,7 +533,7 @@
     <col min="22" max="22" width="20.21875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -502,47 +543,47 @@
       <c r="C1" t="s">
         <v>2</v>
       </c>
-      <c r="D1" s="2" t="s">
+      <c r="D1" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="E1" s="2"/>
-      <c r="F1" s="2" t="s">
+      <c r="E1" s="1"/>
+      <c r="F1" s="1" t="s">
         <v>4</v>
       </c>
-      <c r="G1" s="2"/>
-      <c r="H1" s="2" t="s">
+      <c r="G1" s="1"/>
+      <c r="H1" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="I1" s="2"/>
-      <c r="J1" s="2" t="s">
+      <c r="I1" s="1"/>
+      <c r="J1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="K1" s="2"/>
-      <c r="L1" s="2" t="s">
+      <c r="K1" s="1"/>
+      <c r="L1" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="M1" s="2"/>
-      <c r="N1" s="2" t="s">
+      <c r="M1" s="1"/>
+      <c r="N1" s="1" t="s">
         <v>8</v>
       </c>
-      <c r="O1" s="2"/>
-      <c r="P1" s="2" t="s">
+      <c r="O1" s="1"/>
+      <c r="P1" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="Q1" s="2"/>
-      <c r="R1" s="2" t="s">
+      <c r="Q1" s="1"/>
+      <c r="R1" s="1" t="s">
         <v>10</v>
       </c>
-      <c r="S1" s="2"/>
-      <c r="T1" s="2" t="s">
+      <c r="S1" s="1"/>
+      <c r="T1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="U1" s="2"/>
+      <c r="U1" s="1"/>
       <c r="V1" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="2" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="D2" t="s">
         <v>13</v>
       </c>
@@ -598,7 +639,7 @@
         <v>14</v>
       </c>
     </row>
-    <row r="3" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A3">
         <v>1</v>
       </c>
@@ -618,55 +659,55 @@
         <v>8</v>
       </c>
       <c r="G3" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="H3" t="s">
         <v>18</v>
       </c>
       <c r="I3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J3" t="s">
         <v>18</v>
       </c>
       <c r="K3" t="s">
-        <v>19</v>
+        <v>26</v>
       </c>
       <c r="L3" t="s">
         <v>18</v>
       </c>
       <c r="M3" t="s">
-        <v>19</v>
+        <v>29</v>
       </c>
       <c r="N3" t="s">
         <v>18</v>
       </c>
       <c r="O3" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="P3" t="s">
         <v>18</v>
       </c>
       <c r="Q3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="R3" t="s">
         <v>18</v>
       </c>
       <c r="S3" t="s">
-        <v>19</v>
+        <v>32</v>
       </c>
       <c r="T3" t="s">
         <v>18</v>
       </c>
       <c r="U3" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="V3" t="s">
-        <v>20</v>
+        <v>34</v>
       </c>
     </row>
-    <row r="4" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A4">
         <v>2</v>
       </c>
@@ -680,61 +721,61 @@
         <v>8</v>
       </c>
       <c r="E4" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F4">
         <v>9</v>
       </c>
       <c r="G4" t="s">
-        <v>19</v>
+        <v>23</v>
       </c>
       <c r="H4" t="s">
         <v>18</v>
       </c>
       <c r="I4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J4" t="s">
         <v>18</v>
       </c>
       <c r="K4" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="L4" t="s">
         <v>18</v>
       </c>
       <c r="M4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N4" t="s">
         <v>18</v>
       </c>
       <c r="O4" t="s">
-        <v>19</v>
+        <v>30</v>
       </c>
       <c r="P4" t="s">
         <v>18</v>
       </c>
       <c r="Q4" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="R4" t="s">
         <v>18</v>
       </c>
       <c r="S4" t="s">
-        <v>19</v>
+        <v>33</v>
       </c>
       <c r="T4" t="s">
         <v>18</v>
       </c>
       <c r="U4" t="s">
-        <v>19</v>
-      </c>
-      <c r="V4" s="1" t="s">
-        <v>20</v>
+        <v>25</v>
+      </c>
+      <c r="V4" t="s">
+        <v>34</v>
       </c>
     </row>
-    <row r="5" spans="1:22" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:22" ht="15" x14ac:dyDescent="0.2">
       <c r="A5">
         <v>3</v>
       </c>
@@ -748,62 +789,59 @@
         <v>9</v>
       </c>
       <c r="E5" t="s">
-        <v>19</v>
+        <v>21</v>
       </c>
       <c r="F5">
         <v>8</v>
       </c>
       <c r="G5" t="s">
-        <v>19</v>
+        <v>24</v>
       </c>
       <c r="H5" t="s">
         <v>18</v>
       </c>
       <c r="I5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="J5" t="s">
         <v>18</v>
       </c>
       <c r="K5" t="s">
-        <v>19</v>
+        <v>28</v>
       </c>
       <c r="L5" t="s">
         <v>18</v>
       </c>
       <c r="M5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="N5" t="s">
         <v>18</v>
       </c>
       <c r="O5" t="s">
-        <v>19</v>
+        <v>31</v>
       </c>
       <c r="P5" t="s">
         <v>18</v>
       </c>
       <c r="Q5" t="s">
-        <v>19</v>
+        <v>25</v>
       </c>
       <c r="R5" t="s">
         <v>18</v>
       </c>
       <c r="S5" t="s">
-        <v>19</v>
+        <v>27</v>
       </c>
       <c r="T5" t="s">
         <v>18</v>
       </c>
       <c r="U5" t="s">
-        <v>19</v>
-      </c>
-      <c r="V5" s="1" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:22" x14ac:dyDescent="0.2">
-      <c r="V6" s="1"/>
+        <v>25</v>
+      </c>
+      <c r="V5" t="s">
+        <v>34</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="9">

</xml_diff>